<commit_message>
"v0.5, finish wrappers, process datagrame and upload to mongo cloud"
</commit_message>
<xml_diff>
--- a/Wrappers/Jokes.xlsx
+++ b/Wrappers/Jokes.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mh5JJJ6j6U3ke3Tu4l0jh/15eTlRA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhfAsm9VRaimg3/bj+MkxNRQsxJ+g=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Joke</t>
   </si>
@@ -30,190 +30,158 @@
     <t>Van dos y se cae el del medio</t>
   </si>
   <si>
-    <t>Teacher: "Kids, what does the chicken give you?"Student: "Meat!"Teacher: "Very good! Now what does the pig give you?"Student: "Bacon!"Teacher: "Great! And what does the fat cow give you?"Student: "Homework!"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mi nutricionista me dice : Eres lo que comes.
-Me quedé pensando: vivo comiendo chocolates, pastas, pizzas, hot-dogs, helados, churros y otras cositas...
-Así que he llegado a la conclusión de que soy  deliciosa.
+    <t>My friend thinks he is smart. He told me an onion is the only food that makes you cry, so I threw a coconut at his face.</t>
+  </si>
+  <si>
+    <t>Primer acto: Hay una O
+Segundo acto: Hay un hombre limpiando la O
+Tercer acto: Esta el mismo hombre limpiando la O
+¿Cómo se llama la obra?
+Las O limpiadas</t>
+  </si>
+  <si>
+    <t>What happens to a frog's car when it breaks down?It gets toad away.</t>
+  </si>
+  <si>
+    <t>Los hombres son como los pájaros, vienen cagan y se van.
+Los hombres son como los taxis, nunca viene el que quieres.</t>
+  </si>
+  <si>
+    <t>Q: Is Google male or female? A: Female, because it doesn't let you finish a sentence before making a suggestion.</t>
+  </si>
+  <si>
+    <t>Do you speak English?
+¿Cómo dice usted?
+Do you speak english?
+¡No lo entiendo!
+Le pregunto que si usted habla Inglés.
+¡Ah sí, perfectamente!</t>
+  </si>
+  <si>
+    <t>Q: What did the duck say when he bought lipstick?A: "Put it on my bill."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Cómo se dice hazme reír en Ärabe?
+Hasmejaja.
+¿Cómo se dice lluvia en Árabe?
+Tevamoja.
+¿Cómo se dice comida rápida en Chino?
+Yatá.
 </t>
   </si>
   <si>
-    <t>My friend thinks he is smart. He told me an onion is the only food that makes you cry, so I threw a coconut at his face.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le dice por teléfono una mujer a su esposo: 
-Gordo, perdóname te di las pastillas para los nervios en lugar de las de la diarrea, 
-¿cómo estás?
-Cagado....,  pero tranquilo.... 
+    <t>¿Cómo se dice pobre en Japonés-Chino?
+Chin unchentavo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Mamá, cómo nací yo?
+Ay hijito, pues yo hice un viaje y llegué a un hermoso jardín lleno de flores, entonces escogí un lindo botón.  
+¡Mamá! ¡Sólo quiero saber si fue parto normal o cesárea!
 </t>
   </si>
   <si>
-    <t>What happens to a frog's car when it breaks down?It gets toad away.</t>
-  </si>
-  <si>
-    <t>Una chica romántica le envió un mensaje de texto a su amado diciendo: 
-Si estás durmiendo, envíame tu sueño. 
-Si lloras, envíame tus lágrimas. 
-Si estás sonriendo, ¡envíame tu felicidad!
-Su amado al leer el mensaje  decidió responderle inmediatamente:
-Estoy en el baño.</t>
-  </si>
-  <si>
-    <t>Is Google male or female?. Female, because it doesn't let you finish a sentence before making a suggestion.</t>
-  </si>
-  <si>
-    <t>¿Qué es un Magochicero?
-Un tipo que es hechicero y mago.</t>
-  </si>
-  <si>
-    <t>Kid 1: "Hey, I bet you're still a virgin." Kid 2: "Yeah, I was a virgin until last night ." Kid 1: "As if." Kid 2: "Yeah, just ask your sister." Kid 1: "I don't have a sister." Kid 2: "You will in about nine months."</t>
-  </si>
-  <si>
-    <t>¿Cuánto dura una bala en atravesar el cerebro de un hombre?
-Tres días, de aquí a que se encuentre el cerebro...</t>
-  </si>
-  <si>
-    <t>What did the duck say when he bought lipstick?. "Put it on my bill."</t>
-  </si>
-  <si>
-    <t>Cuando el cerebro de un hombre mide un centímetro, ¿Qué es lo que pasa?
-Está inflamado.</t>
-  </si>
-  <si>
-    <t>A teacher asked her students to use the word "beans" in a sentence. "My father grows beans," said one girl. "My mother cooks beans," said a boy. A third student spoke up, "We are all human beans."</t>
-  </si>
-  <si>
-    <t>Cuando los hombres cagan piensan y cuando piensan la cagan.</t>
-  </si>
-  <si>
-    <t>Have you heard about the new restaurant called Karma? There’s no menu; you get what you deserve.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profesores.
-A ver Pepito . ¿dónde está el sujeto en esta oración.?
-El enriqueció de la noche a la mañana 
-Pepito: Seguramente en la política señorita.
+    <t>Pepito le pregunta a la mamá:
+Oye mami, ¿Los chocolates caminan?
+No pepito, los chocolates no caminan.
+Y Pepito le dice:
+Pues creo que me comí una cucaracha.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el colmo de saturno?
+Que tenga anillos y no tenga dedos.</t>
+  </si>
+  <si>
+    <t>Q: Why did the witches' team lose the baseball game? A: Their bats flew away.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este era un bebe tan feo, que cuando nació, el médico dijo:
+Señora, lo tiramos al aire, y si vuela, es murciélago.
 </t>
   </si>
   <si>
-    <t>A lot of people cry when they cut an onion. The trick is not to form an emotional bond.</t>
-  </si>
-  <si>
-    <t>¿En qué se parecen las mujeres a los huracanes?
-En que llegan fuertes y salvajes y se van con tu carro y tu casa.</t>
-  </si>
-  <si>
-    <t>What has more lives than a cat?. A frog because it croaks every night.</t>
-  </si>
-  <si>
-    <t>Un Atlante entra a una tienda y le dice al vendedor:
-Me vende este televisor.
-¡No!, aquí no se atienden atlantes.
-El atlante sorprendido le pregunta al vendedor:
-¿Cómo sabe usted que soy atlante?
-Y el vendedor le responde:
-Muy fácil, este no es un televisor, es un horno de microondas.</t>
-  </si>
-  <si>
-    <t>Does anyone remember the Swatch, a watch made in Switzerland? Thank god Croatia didn't come up with the idea first. Just imagine if someone were to ask you what time is it? "Oh pardon me while I look at my crotch."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En una ocasión había muchas personas reunidas en una casa y pasó por aquel lugar un conocido de la familia y preguntó... 
-- ¿Qué pasó compadre?... ¿murió alguien? 
-- Si, mi burro mató a mi suegra de una patada. 
-- ¿Y toda esa gente conocía a tu suegra? 
-- No... ¡Vinieron a comprar el burro!
-</t>
-  </si>
-  <si>
-    <t>What do you call a cow that just gave birth?. Decalfeinated.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un padre molesto por  el rendimiento escolar de su hijo le dice:
-Hijo  Si repruebas el examen de mañana  olvídate  que soy tu padre.
-Al día siguiente el padre le pregunta:
-Hijo, ¿Cómo te fue en el examen?
-Y el hijo muy sorprendido le responde:
-Y tú ¿quién eres?
-</t>
-  </si>
-  <si>
-    <t>Son: "Dad, when will I be old enough so I don't have to ask mom for her permission to go out?" Dad: "Son, even I haven't grown old enough to go out without her permission!"</t>
-  </si>
-  <si>
-    <t>¿Qué hace una neurona en la cabeza de un hombre?
-¡Turismo!</t>
-  </si>
-  <si>
-    <t>Why is a baseball game a good place to go on a hot day? Because there are lots of fans.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profesora de lenguaje
-A ver niños si yo digo:  encontré novio.
-¿dónde está el sujeto?
-Pepito:  ¡espero que comprando anteojos profesora.!
-</t>
-  </si>
-  <si>
-    <t>If a man opens the car door for his wife, you can be sure of one thing: either the car is new or the wife.</t>
-  </si>
-  <si>
-    <t>En un carro iba una pareja de casados pero iban peleados, al pasar frente a una granja el novio vio unos cochinitos y le dijo a la mujer:
-¿Familiares tuyos?
-Y ella le contestó: 
-¡Sí, mis suegros!</t>
-  </si>
-  <si>
-    <t>A man called his child's doctor, "Hello! My son just snatched my pen when I was writing and swallowed it. What should I do?" The doctor replied, "Until I can come over, write with another pen."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La maestra le pregunta a Pepito:
-Pepito, ¿Cómo se dice en ingles: el gato se cayó en el agua y se ahogo ?.
-Fácil maestra: The cat cataplum in the water glugluglu and not mas miau miau.
-</t>
-  </si>
-  <si>
-    <t>Why did Captain Kirk go in to the ladies room?. Because he wanted to go where no man had gone before.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Llega un niño con su papá y le dice: papá, papá es cierto que al hombre se le conquista por el estomago.
-Responde el papá: sí yo me case con tu mamá cuando le empezó a crecer el suyo.
-</t>
-  </si>
-  <si>
-    <t>A disciple went to his master and said, "I have served you faithfully for ten years. Now I have a wish: give me something to eat which will never end." His master said, "Here, have some chewing gum."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La cerveza fomenta los poderes  de telekinesis
-Cuando te dicen que la leche te hace fuerte. ¿Has probado tomarte 10 vasos de leche y tratar de mover una  pared?. La verdad no podrás moverla_x0085_
-Pero si tomas 10 vasos de cerveza, verás como logras que la pared se mueva sola
-</t>
-  </si>
-  <si>
-    <t>Man: What would you do if I won the lottery?. Woman: Take half and leave!. Man: Well, I won 20 bucks, here's 10, now get out!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un señor manda su ropa interior a la lavandería y pone una nota: 
-- Usar más jabón en los bóxer... 
-Cuando recoge su ropa encuentra una nota que decía: 
-- Usar más papel higienico... 
-</t>
-  </si>
-  <si>
-    <t>What says "Eoo?" A cow with no lips.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En un Censo.
-Estaba la encuestadora en una casa haciendo la encuesta y pregunta:
-¿Su nombre?
-Adán.
-¿El nombre de su esposa?
-Eva.
-¡Increíble! ¿Por casualidad la serpiente también vive aquí?
-Sí, un momento. 
-¡Sueeegraaaa, la BUSCAN !
-</t>
+    <t>Q: Why couldn't the leopard play hide and seek? A: Because he was always spotted.</t>
+  </si>
+  <si>
+    <t>Oye Manolo, se ha cortado la luz.
+Pues, ponle una curita.</t>
+  </si>
+  <si>
+    <t>Q: Can a kangaroo jump higher than the Empire State Building? A: Of course. The Empire State Building can't jump.</t>
+  </si>
+  <si>
+    <t>Esta era una vez un niño que le dice a su mamá:
+Mamá, mamá, ¿Qué día nací yo?
+Su mamá responde:
+El 15 de abril, hijo.
+El niño responde:
+¡Ah, que coincidencia, nací el mismo día de mi cumpleaños!</t>
+  </si>
+  <si>
+    <t>Q: Why was six scared of seven? A: Because seven "ate" nine.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el colmo de un fotógrafo?
+Que su hijo se le rebele.</t>
+  </si>
+  <si>
+    <t>Q: What starts with E, ends with E, and has only 1 letter in it? A: Envelope.</t>
+  </si>
+  <si>
+    <t>¿Cómo se dice 99 en chino?
+Cachichien.</t>
+  </si>
+  <si>
+    <t>Q: Why couldn't the blonde add 10 + 5 on a calculator? A: She couldn't find the "10" button.</t>
+  </si>
+  <si>
+    <t>Un hombre va a un abogado.
+- Y usted cuanto cobra por una consulta rápida ?
+- 10.000 pesetas por tres preguntas.
+- Vaya, es un poco caro, no ?
+- Sí ... y dígame, cuál es su tercera pregunta ?</t>
+  </si>
+  <si>
+    <t>Instead of "the John," I call my toilet "the Jim." That way it sounds better when I say I go to the Jim first thing every morning.</t>
+  </si>
+  <si>
+    <t>¿Qué es algo verde y peligroso?
+Una ranita con metralleta.</t>
+  </si>
+  <si>
+    <t>Q: Did you hear about the kidnapping at school? A: It's okay. He woke up.</t>
+  </si>
+  <si>
+    <t>Mamá, mamá, ¡En la escuela me dicen Back Street Boy!
+¿Quién te dice así?
+¡Every body!</t>
+  </si>
+  <si>
+    <t>Q: Why did the can crusher quit his job? A: Because it was soda pressing.</t>
+  </si>
+  <si>
+    <t>La sabiduría me persigue, pero yo voy más rápido.</t>
+  </si>
+  <si>
+    <t>Math Teacher: "If I have 5 bottles in one hand and 6 in the other hand, what do I have?" Student: "A drinking problem."</t>
+  </si>
+  <si>
+    <t>¡Mamá, mamá, en el colegio no saben decir mi nombre!
+La mamá le responde:
+¡Cállate Bonifacioestuladicolofeilo que no me dejas oir las noticias!</t>
+  </si>
+  <si>
+    <t>My friend told me he had the body of a Greek god. I had to explain to him that Buddha is not Greek.</t>
+  </si>
+  <si>
+    <t>¿Cuáles son las medidas perfectas de un hombre?
+80-2-80, 80 años, 2 infartos y 80 millones de euros en la cuenta del banco.</t>
+  </si>
+  <si>
+    <t>Q: Why did Adele cross the road? A: To sing, "Hello from the other side!"</t>
+  </si>
+  <si>
+    <t>¿Qué es el tiempo sin ti?
+¡EMPO!</t>
   </si>
 </sst>
 </file>
@@ -523,7 +491,7 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -534,7 +502,7 @@
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -553,7 +521,7 @@
       <c r="A6" s="1">
         <v>4.0</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -565,21 +533,21 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
         <v>6.0</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -587,21 +555,21 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
         <v>8.0</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -609,21 +577,21 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
         <v>10.0</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>22</v>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
@@ -631,21 +599,21 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
         <v>12.0</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>26</v>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15">
@@ -653,21 +621,21 @@
         <v>13.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
         <v>14.0</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17">
@@ -675,10 +643,10 @@
         <v>15.0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18">
@@ -686,21 +654,21 @@
         <v>16.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
         <v>17.0</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>36</v>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
@@ -708,32 +676,32 @@
         <v>18.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1">
         <v>19.0</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>40</v>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1">
         <v>20.0</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>42</v>
+      <c r="B22" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1"/>

</xml_diff>